<commit_message>
Fix Unserved Report Viewing and PO Report Viewing
</commit_message>
<xml_diff>
--- a/RFQ.xlsx
+++ b/RFQ.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>CENTRAL NEGROS POWER RELIABILITY, INC.</t>
   </si>
@@ -41,34 +41,37 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>November 27, 2019</t>
+    <t>October 29, 2019</t>
   </si>
   <si>
     <t>RFQ No.:</t>
   </si>
   <si>
-    <t>201911-1028-A</t>
+    <t>201910-1016-R</t>
   </si>
   <si>
     <t>Urg:</t>
   </si>
   <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>Supplier:</t>
   </si>
   <si>
-    <t>Bacolod Sure Computer, Inc.</t>
+    <t>Bacolod Steel Center Corporation</t>
   </si>
   <si>
     <t>Tel. No.:</t>
   </si>
   <si>
-    <t>(034) 435-1949</t>
+    <t>435-2721-25</t>
   </si>
   <si>
     <t>PR No.:</t>
   </si>
   <si>
-    <t>TRA19-1010</t>
+    <t>OPE19-1016</t>
   </si>
   <si>
     <t>No.</t>
@@ -89,10 +92,10 @@
     <t>Unit Price</t>
   </si>
   <si>
-    <t>pc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB cord, </t>
+    <t>sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perforated Sheet, Stainless Steel, Round Holes, Hole Diameter: 5mm, Thickness: 1mm, </t>
   </si>
   <si>
     <t xml:space="preserve">1. Quotation must be submitted on or before </t>
@@ -137,10 +140,10 @@
     <t>Approved By:</t>
   </si>
   <si>
-    <t>Prency Francisco</t>
-  </si>
-  <si>
-    <t>Syndey Sinoro</t>
+    <t>Kervic Binas</t>
+  </si>
+  <si>
+    <t>Maylen Cabaylo</t>
   </si>
   <si>
     <t>Ma. Milagros Arana</t>
@@ -267,14 +270,14 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>-285750</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="333375" cy="333375"/>
+    <xdr:ext cx="952500" cy="952500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Sample image" descr="Sample image"/>
+        <xdr:cNvPr id="1" name="Logo" descr="Logo"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -688,55 +691,57 @@
       <c r="I9" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="8"/>
+      <c r="J9" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:11">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D10" s="8"/>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:11">
       <c r="F11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H11" s="8"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
@@ -748,10 +753,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -763,37 +768,37 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -801,7 +806,7 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -809,25 +814,25 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -840,13 +845,13 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit new signatories in PO and RFD
</commit_message>
<xml_diff>
--- a/RFQ.xlsx
+++ b/RFQ.xlsx
@@ -15,24 +15,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
-  <si>
-    <t>CENTRAL NEGROS POWER RELIABILITY, INC.</t>
-  </si>
-  <si>
-    <t>TIN No. HERE</t>
-  </si>
-  <si>
-    <t>Office: 88 Corner Rizal-Mabini Sts., Bacolod City</t>
-  </si>
-  <si>
-    <t>Tel. No.: (034) 435-1932/476-7382</t>
-  </si>
-  <si>
-    <t>Telefax: (034) 435-1932</t>
-  </si>
-  <si>
-    <t>Plant Site: Purok San Jose, Barangay Calumangan, Bago City</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+  <si>
+    <t>CALAPAN POWER GENERATION CORPORATION</t>
+  </si>
+  <si>
+    <t>TIN No. 008-158-746-000</t>
+  </si>
+  <si>
+    <t>NPC Bldg.Sta Isabel,Calapan City Oriental Mindoro</t>
+  </si>
+  <si>
+    <t>Tel. No.: 738-0186</t>
+  </si>
+  <si>
+    <t>Telefax: 738-0186</t>
   </si>
   <si>
     <t>REQUEST FOR QUOTATION</t>
@@ -41,13 +38,13 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>February 3, 2021</t>
+    <t>April 30, 2020</t>
   </si>
   <si>
     <t>RFQ No.:</t>
   </si>
   <si>
-    <t>ITB21-1003-A</t>
+    <t>202004-1034-B</t>
   </si>
   <si>
     <t>Urg:</t>
@@ -56,19 +53,19 @@
     <t>Supplier:</t>
   </si>
   <si>
-    <t>Pinamalayan Hyper Market</t>
+    <t>Lubri-Chem Philippines Distributors, Inc.</t>
   </si>
   <si>
     <t>Tel. No.:</t>
   </si>
   <si>
-    <t>034 659 6568</t>
+    <t>364-8484, 364-2703</t>
   </si>
   <si>
     <t>PR No.:</t>
   </si>
   <si>
-    <t>ITB21-1003</t>
+    <t>OPC20-1086</t>
   </si>
   <si>
     <t>No.</t>
@@ -89,25 +86,13 @@
     <t>Unit Price</t>
   </si>
   <si>
-    <t>bot/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hand Soap, 100ml, </t>
-  </si>
-  <si>
-    <t>roll/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tissue, </t>
-  </si>
-  <si>
-    <t>gal/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alcohol, </t>
-  </si>
-  <si>
-    <t>1. Quotation must be submitted on or before 2021-02-03</t>
+    <t>drums</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shell Argina S4, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Quotation must be submitted on or before </t>
   </si>
   <si>
     <t>Please Fill - Up :</t>
@@ -149,13 +134,10 @@
     <t>Approved By:</t>
   </si>
   <si>
-    <t>Hennelen Tanan</t>
-  </si>
-  <si>
-    <t>Elaine Anne Y. dela Cruz</t>
-  </si>
-  <si>
-    <t>Enrico Brian Ani</t>
+    <t>Myra Aceveda</t>
+  </si>
+  <si>
+    <t>Myra A. Aceveda</t>
   </si>
 </sst>
 </file>
@@ -599,7 +581,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="J9" sqref="J9"/>
@@ -663,9 +645,7 @@
       <c r="H5"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6"/>
@@ -674,7 +654,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7"/>
       <c r="E7"/>
@@ -684,71 +664,71 @@
     </row>
     <row r="9" spans="1:11">
       <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>8</v>
       </c>
       <c r="D9" s="8"/>
       <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>10</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:11">
       <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="D10" s="8"/>
       <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:11">
       <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="H11" s="8"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>21</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K13" s="10"/>
     </row>
@@ -757,13 +737,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="3">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -773,134 +753,92 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="2">
-        <v>2</v>
-      </c>
-      <c r="B15" s="3">
-        <v>10</v>
-      </c>
-      <c r="C15" s="4" t="s">
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="4" t="s">
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="2">
-        <v>3</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" t="s">
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="5" t="s">
+      <c r="E24" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="5" t="s">
+      <c r="H24" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4" t="s">
+    </row>
+    <row r="25" spans="1:11">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="E26" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" t="s">
-        <v>42</v>
-      </c>
       <c r="H26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" t="s">
-        <v>45</v>
-      </c>
-      <c r="H28" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -909,12 +847,6 @@
     <mergeCell ref="D14:G14"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="J14:K14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="C3:H3"/>

</xml_diff>